<commit_message>
Ultimos ajustes para la entrega de diseño
</commit_message>
<xml_diff>
--- a/Informes/Informe_3/Encuesta.xlsx
+++ b/Informes/Informe_3/Encuesta.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="18915" windowHeight="7230"/>
+    <workbookView xWindow="360" yWindow="80" windowWidth="20420" windowHeight="11480"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Encuesta Perfil Solicitante</t>
   </si>
@@ -187,13 +192,22 @@
   </si>
   <si>
     <t>Los graficos en los resumen permiten una mejor visualizacion de la infofrmacion</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>} &amp; {} &amp;{} &amp;{} &amp; {} &amp; {} \\</t>
+  </si>
+  <si>
+    <t>Encuesta Perfil Jefe de Departamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +227,22 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,15 +275,171 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -262,8 +448,167 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="157">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,58 +910,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="96.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="96.5" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15">
       <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="C10" t="s">
         <v>2</v>
       </c>
@@ -624,24 +969,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="C11">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
@@ -649,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2</v>
       </c>
@@ -657,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>3</v>
       </c>
@@ -665,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>4</v>
       </c>
@@ -673,7 +1018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>5</v>
       </c>
@@ -681,7 +1026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>6</v>
       </c>
@@ -689,308 +1034,418 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15">
       <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3">
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="3">
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="3">
         <v>5</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <v>6</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3">
+        <v>7</v>
+      </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>8</v>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="3">
+        <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>9</v>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="3">
+        <v>10</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>10</v>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="3">
+        <v>11</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>11</v>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="3">
+        <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>12</v>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="3">
+        <v>13</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>13</v>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="3">
+        <v>14</v>
       </c>
       <c r="B33" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>14</v>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3">
+        <v>15</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>15</v>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3">
+        <v>16</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3">
+        <v>17</v>
+      </c>
       <c r="B36" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3">
+        <v>18</v>
+      </c>
       <c r="B37" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15">
+      <c r="A40" s="3">
+        <v>1</v>
+      </c>
       <c r="B40" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
+    <row r="41" spans="1:3">
+      <c r="A41" s="8">
+        <v>2</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2</v>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8">
+        <v>3</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>3</v>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3">
+        <v>4</v>
       </c>
       <c r="B43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
+      <c r="A44" s="8">
+        <v>5</v>
+      </c>
       <c r="B44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>4</v>
+    <row r="45" spans="1:3">
+      <c r="A45" s="8">
+        <v>6</v>
       </c>
       <c r="B45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>5</v>
+    <row r="46" spans="1:3">
+      <c r="A46" s="3">
+        <v>7</v>
       </c>
       <c r="B46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>6</v>
+    <row r="47" spans="1:3">
+      <c r="A47" s="8">
+        <v>8</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>7</v>
+    <row r="48" spans="1:3">
+      <c r="A48" s="8">
+        <v>9</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>8</v>
+    <row r="49" spans="1:2">
+      <c r="A49" s="3">
+        <v>10</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>9</v>
+    <row r="50" spans="1:2">
+      <c r="A50" s="8">
+        <v>11</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
+      <c r="A51" s="8">
+        <v>12</v>
+      </c>
       <c r="B51" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
+      <c r="A52" s="3">
+        <v>13</v>
+      </c>
       <c r="B52" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
+      <c r="A53" s="8">
+        <v>14</v>
+      </c>
       <c r="B53" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
+      <c r="A54" s="8">
+        <v>15</v>
+      </c>
       <c r="B54" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
+      <c r="A55" s="3">
+        <v>16</v>
+      </c>
       <c r="B55" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
+      <c r="A56" s="8">
+        <v>17</v>
+      </c>
       <c r="B56" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
+      <c r="A57" s="8">
+        <v>18</v>
+      </c>
       <c r="B57" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
+      <c r="A58" s="3">
+        <v>19</v>
+      </c>
       <c r="B58" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
+      <c r="A59" s="3">
+        <v>20</v>
+      </c>
       <c r="B59" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="15">
       <c r="B62" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="B64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2">
       <c r="B66" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2">
       <c r="B67" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2">
       <c r="B68" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1000,9 +1455,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1012,8 +1472,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>